<commit_message>
Dispatcher update - Get return from Taxsolver, save it into a excel file and upload to the queue. Need some tests and prepare unit tests as well
</commit_message>
<xml_diff>
--- a/STS IR Bot Dispatcher/Data/Config.xlsx
+++ b/STS IR Bot Dispatcher/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://taxwarellc-my.sharepoint.com/personal/nahuel_delacruz_sovos_com/Documents/Documents/UiPath/PRC_Taxpayer_v2/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://taxwarellc-my.sharepoint.com/personal/nahuel_delacruz_sovos_com/Documents/Desktop/Nahuel/Projects/STS Internal Review bot/STS IR Bot Dispatcher/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B41780E6-D387-481F-8F75-0347AEEB2D36}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A75635CC-6DDF-4ADD-B28A-7424A61D6792}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="62">
   <si>
     <t>Name</t>
   </si>
@@ -95,104 +95,121 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
+    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction succesful.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with business exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with application exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Calling Get Transaction Data.</t>
+  </si>
+  <si>
+    <t>OrchestratorAssetFolder</t>
+  </si>
+  <si>
+    <t>OrchestratorQueueFolder</t>
+  </si>
+  <si>
+    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
+  </si>
+  <si>
+    <t>MaxConsecutiveSystemExceptions</t>
+  </si>
+  <si>
+    <t>ExceptionMessage_ConsecutiveErrors</t>
+  </si>
+  <si>
+    <t>RetryNumberGetTransactionItem</t>
+  </si>
+  <si>
+    <t>RetryNumberSetTransactionStatus</t>
+  </si>
+  <si>
+    <t>Error message in case MaxConsecutiveSystemExceptions number is reached.</t>
+  </si>
+  <si>
+    <t>The number of times Get Transaction Item activity is retried in case of an exception. Must be an integer &gt;= 1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
+  </si>
+  <si>
+    <t>ShouldMarkJobAsFaulted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveSystemExceptions is reached, the job is stopped. To disable this feature, set the value to 0. </t>
+  </si>
+  <si>
+    <t>Must be TRUE or FALSE. If the value is TRUE and an error occurs in Initialization state or the MaxConsecutiveSystemExceptions is reached, the job is marked as Faulted.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
+  </si>
+  <si>
+    <t>SUT/STS</t>
+  </si>
+  <si>
+    <t>taxSolverBrowserCredential</t>
+  </si>
+  <si>
+    <t>TaxSolver browser credential</t>
+  </si>
+  <si>
+    <t>taxSolverApplicationCredential</t>
+  </si>
+  <si>
+    <t>TaxSolver application credential</t>
+  </si>
+  <si>
+    <t>netDriveCredential</t>
+  </si>
+  <si>
+    <t>Net drive credential</t>
+  </si>
+  <si>
+    <t>netDriveLetter</t>
+  </si>
+  <si>
+    <t>Net drive letter</t>
+  </si>
+  <si>
+    <t>netDrivePath</t>
+  </si>
+  <si>
+    <t>Net drive path</t>
+  </si>
+  <si>
+    <t>Internal_Review_Dispatcher</t>
+  </si>
+  <si>
+    <t>Returns Table &lt;DATE&gt;.xlsx</t>
+  </si>
+  <si>
+    <t>PathReturnsTableFilename</t>
+  </si>
+  <si>
+    <t>The filename of the returns table the bot will get from TaxSolver. Include the extension</t>
+  </si>
+  <si>
+    <t>ReturnsFile_WorksheetName</t>
+  </si>
+  <si>
+    <t>Sheet1</t>
+  </si>
+  <si>
+    <t>The worksheet name of the returns file, were the whole return list is saved</t>
+  </si>
+  <si>
     <t>OrchestratorQueueName</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction succesful.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with business exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with application exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Calling Get Transaction Data.</t>
-  </si>
-  <si>
-    <t>OrchestratorAssetFolder</t>
-  </si>
-  <si>
-    <t>OrchestratorQueueFolder</t>
-  </si>
-  <si>
-    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
-  </si>
-  <si>
-    <t>MaxConsecutiveSystemExceptions</t>
-  </si>
-  <si>
-    <t>ExceptionMessage_ConsecutiveErrors</t>
-  </si>
-  <si>
-    <t>RetryNumberGetTransactionItem</t>
-  </si>
-  <si>
-    <t>RetryNumberSetTransactionStatus</t>
-  </si>
-  <si>
-    <t>Error message in case MaxConsecutiveSystemExceptions number is reached.</t>
-  </si>
-  <si>
-    <t>The number of times Get Transaction Item activity is retried in case of an exception. Must be an integer &gt;= 1.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
-  </si>
-  <si>
-    <t>ShouldMarkJobAsFaulted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveSystemExceptions is reached, the job is stopped. To disable this feature, set the value to 0. </t>
-  </si>
-  <si>
-    <t>Must be TRUE or FALSE. If the value is TRUE and an error occurs in Initialization state or the MaxConsecutiveSystemExceptions is reached, the job is marked as Faulted.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
-  </si>
-  <si>
-    <t>TaxSolver- Returns</t>
-  </si>
-  <si>
-    <t>SUT/STS</t>
-  </si>
-  <si>
-    <t>PRC_Taxpayer_Dispatcher</t>
-  </si>
-  <si>
-    <t>taxSolverBrowserCredential</t>
-  </si>
-  <si>
-    <t>TaxSolver browser credential</t>
-  </si>
-  <si>
-    <t>taxSolverApplicationCredential</t>
-  </si>
-  <si>
-    <t>TaxSolver application credential</t>
-  </si>
-  <si>
-    <t>netDriveCredential</t>
-  </si>
-  <si>
-    <t>Net drive credential</t>
-  </si>
-  <si>
-    <t>netDriveLetter</t>
-  </si>
-  <si>
-    <t>Net drive letter</t>
-  </si>
-  <si>
-    <t>netDrivePath</t>
-  </si>
-  <si>
-    <t>Net drive path</t>
+  </si>
+  <si>
+    <t>TaxSolver_Returns</t>
   </si>
 </sst>
 </file>
@@ -269,6 +286,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -570,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -618,10 +639,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -629,13 +650,13 @@
     </row>
     <row r="3" spans="1:26" ht="45">
       <c r="A3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -644,7 +665,7 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>22</v>
@@ -653,41 +674,61 @@
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" t="s">
+        <v>56</v>
+      </c>
+    </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" t="s">
+        <v>59</v>
+      </c>
+    </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1738,18 +1779,18 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1773,7 +1814,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -1795,7 +1836,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1806,7 +1847,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -1817,53 +1858,53 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2847,8 +2888,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2867,7 +2908,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -2897,30 +2938,30 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Commit in relation to performing of the dispatcher and performer process
</commit_message>
<xml_diff>
--- a/STS IR Bot Dispatcher/Data/Config.xlsx
+++ b/STS IR Bot Dispatcher/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://taxwarellc-my.sharepoint.com/personal/nahuel_delacruz_sovos_com/Documents/Desktop/Nahuel/Projects/STS Internal Review bot/STS IR Bot Dispatcher/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martin.martinez\Documents\github-IRBot\STS_InternalReviewBot\STS IR Bot Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A75635CC-6DDF-4ADD-B28A-7424A61D6792}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9629EB71-785D-47BA-A3E7-B3D3B9E82803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="68">
   <si>
     <t>Name</t>
   </si>
@@ -210,6 +210,24 @@
   </si>
   <si>
     <t>TaxSolver_Returns</t>
+  </si>
+  <si>
+    <t>PathTempDirectory</t>
+  </si>
+  <si>
+    <t>the path of the folder where the temporary file will be saved and then used by the performer process</t>
+  </si>
+  <si>
+    <t>C:\Users\martin.martinez\Documents\UiPath\temp</t>
+  </si>
+  <si>
+    <t>TempFile_FileName</t>
+  </si>
+  <si>
+    <t>temp.xlsx</t>
+  </si>
+  <si>
+    <t>the name of the excel file where the data will be stored for later use by the performer process</t>
   </si>
 </sst>
 </file>
@@ -286,10 +304,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -589,17 +603,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="43.5703125" customWidth="1"/>
-    <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="2" max="2" width="48" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="93.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -717,20 +731,40 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A13" t="s">
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
         <v>57</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>58</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" t="s">
+        <v>67</v>
+      </c>
+    </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
@@ -1714,6 +1748,7 @@
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
+    <row r="999" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
New Exceptional Case (Jefferson County) was added
</commit_message>
<xml_diff>
--- a/STS IR Bot Dispatcher/Data/Config.xlsx
+++ b/STS IR Bot Dispatcher/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martin.martinez\Documents\github-IRBot\STS_InternalReviewBot\STS IR Bot Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9629EB71-785D-47BA-A3E7-B3D3B9E82803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A56275-A9E0-413C-960D-2EBDA3C80CF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4335" yWindow="2610" windowWidth="21600" windowHeight="11265" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -605,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1760,7 +1760,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Changes in dispatcher. Customer Account list added. Path of list was hardcoded and it was fixed. update config file
</commit_message>
<xml_diff>
--- a/STS IR Bot Dispatcher/Data/Config.xlsx
+++ b/STS IR Bot Dispatcher/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martin.martinez\Documents\github-IRBot\STS_InternalReviewBot\STS IR Bot Dispatcher\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://taxwarellc-my.sharepoint.com/personal/nahuel_delacruz_sovos_com/Documents/Desktop/Nahuel/Projects/STS Internal Review bot/STS IR Bot Dispatcher/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A56275-A9E0-413C-960D-2EBDA3C80CF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{20A56275-A9E0-413C-960D-2EBDA3C80CF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B24125B-2D4B-4EF0-8EB3-9758C2FF37CE}"/>
   <bookViews>
-    <workbookView xWindow="4335" yWindow="2610" windowWidth="21600" windowHeight="11265" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="70">
   <si>
     <t>Name</t>
   </si>
@@ -218,9 +218,6 @@
     <t>the path of the folder where the temporary file will be saved and then used by the performer process</t>
   </si>
   <si>
-    <t>C:\Users\martin.martinez\Documents\UiPath\temp</t>
-  </si>
-  <si>
     <t>TempFile_FileName</t>
   </si>
   <si>
@@ -228,6 +225,15 @@
   </si>
   <si>
     <t>the name of the excel file where the data will be stored for later use by the performer process</t>
+  </si>
+  <si>
+    <t>C:\Users\&lt;USERNAME&gt;\Documents\UiPath\temp</t>
+  </si>
+  <si>
+    <t>Data\Customer Account List.xlsx</t>
+  </si>
+  <si>
+    <t>PathCustomerNameList</t>
   </si>
 </sst>
 </file>
@@ -603,10 +609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z999"/>
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -733,39 +739,46 @@
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
         <v>62</v>
       </c>
-      <c r="B12" t="s">
-        <v>64</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="B13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A14" t="s">
-        <v>57</v>
-      </c>
-      <c r="B14" t="s">
-        <v>58</v>
-      </c>
-      <c r="C14" t="s">
-        <v>59</v>
-      </c>
-    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" t="s">
         <v>65</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C16" t="s">
         <v>66</v>
       </c>
-      <c r="C15" t="s">
-        <v>67</v>
-      </c>
     </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
@@ -1749,6 +1762,7 @@
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
     <row r="999" ht="14.25" customHeight="1"/>
+    <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1760,8 +1774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Copy Input files from P drive. Delete old input files. New rows added in gitignore file
</commit_message>
<xml_diff>
--- a/STS IR Bot Dispatcher/Data/Config.xlsx
+++ b/STS IR Bot Dispatcher/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://taxwarellc-my.sharepoint.com/personal/nahuel_delacruz_sovos_com/Documents/Desktop/Nahuel/Projects/STS Internal Review bot/STS IR Bot Dispatcher/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{20A56275-A9E0-413C-960D-2EBDA3C80CF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B24125B-2D4B-4EF0-8EB3-9758C2FF37CE}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{20A56275-A9E0-413C-960D-2EBDA3C80CF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E15444AD-EF3C-4031-982B-8DAB0123991D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7125" yWindow="4335" windowWidth="21600" windowHeight="11265" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="80">
   <si>
     <t>Name</t>
   </si>
@@ -234,6 +234,36 @@
   </si>
   <si>
     <t>PathCustomerNameList</t>
+  </si>
+  <si>
+    <t>ListInputFiles</t>
+  </si>
+  <si>
+    <t>PathOtherDeductionsList,PathMarginsList,PathCustomerNameList</t>
+  </si>
+  <si>
+    <t>Constant names (from this sheet) of each input file that must be copied from the P drive</t>
+  </si>
+  <si>
+    <t>PathOtherDeductionsList</t>
+  </si>
+  <si>
+    <t>PathPDriveFolder</t>
+  </si>
+  <si>
+    <t>\\somproddfs1.prod.sovos.org\depts\TaxSolver Files</t>
+  </si>
+  <si>
+    <t>PathMarginsList</t>
+  </si>
+  <si>
+    <t>Data\Margins List.xlsx</t>
+  </si>
+  <si>
+    <t>Data\Other Deductions List.xlsx</t>
+  </si>
+  <si>
+    <t>\\somproddfs1.prod.sovos.org\depts\TaxReturnOutSourcing\Preparer\UIPathPublish\IR Bot Temp Files\InputFiles</t>
   </si>
 </sst>
 </file>
@@ -265,12 +295,24 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -285,7 +327,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -295,6 +337,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -609,10 +653,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -726,23 +770,26 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A11" t="s">
-        <v>55</v>
-      </c>
-      <c r="B11" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" t="s">
-        <v>56</v>
+    <row r="11" spans="1:26" s="5" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A11" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="B12" t="s">
-        <v>68</v>
+        <v>54</v>
+      </c>
+      <c r="C12" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
@@ -756,45 +803,76 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A15" t="s">
+    <row r="14" spans="1:26" s="6" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A14" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" s="5" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A15" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" s="6" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A16" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A17" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A19" t="s">
         <v>57</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B19" t="s">
         <v>58</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C19" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A16" t="s">
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
         <v>64</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B20" t="s">
         <v>65</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C20" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -1763,6 +1841,10 @@
     <row r="998" ht="14.25" customHeight="1"/>
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
+    <row r="1001" ht="14.25" customHeight="1"/>
+    <row r="1002" ht="14.25" customHeight="1"/>
+    <row r="1003" ht="14.25" customHeight="1"/>
+    <row r="1004" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1774,8 +1856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1836,7 +1918,7 @@
         <v>31</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
commit to add new path for P drive for specific user
</commit_message>
<xml_diff>
--- a/STS IR Bot Dispatcher/Data/Config.xlsx
+++ b/STS IR Bot Dispatcher/Data/Config.xlsx
@@ -1,28 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://taxwarellc-my.sharepoint.com/personal/nahuel_delacruz_sovos_com/Documents/Desktop/Nahuel/Projects/STS Internal Review bot/STS IR Bot Dispatcher/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martin.martinez\Documents\github-IRBot\STS_InternalReviewBot\STS IR Bot Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{20A56275-A9E0-413C-960D-2EBDA3C80CF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E15444AD-EF3C-4031-982B-8DAB0123991D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F3C4234-F726-4C81-854F-2DAAEEC57946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7125" yWindow="4335" windowWidth="21600" windowHeight="11265" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
     <sheet name="Constants" sheetId="2" r:id="rId2"/>
     <sheet name="Assets" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="82">
   <si>
     <t>Name</t>
   </si>
@@ -264,6 +277,12 @@
   </si>
   <si>
     <t>\\somproddfs1.prod.sovos.org\depts\TaxReturnOutSourcing\Preparer\UIPathPublish\IR Bot Temp Files\InputFiles</t>
+  </si>
+  <si>
+    <t>PathDifferentPDriveFolder</t>
+  </si>
+  <si>
+    <t>\\10.250.52.158\Depts\TaxReturnOutSourcing\Preparer\UIPathPublish\IR Bot Temp Files\InputFiles</t>
   </si>
 </sst>
 </file>
@@ -653,10 +672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1004"/>
+  <dimension ref="A1:Z1005"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -811,57 +830,67 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:26" s="5" customFormat="1" ht="14.25" customHeight="1">
+    <row r="15" spans="1:26" s="6" customFormat="1" ht="14.25" customHeight="1">
       <c r="A15" s="5" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:26" s="6" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A16" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>77</v>
+    <row r="16" spans="1:26" s="5" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A16" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
       <c r="A17" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A18" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B18" s="6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A19" t="s">
-        <v>57</v>
-      </c>
-      <c r="B19" t="s">
-        <v>58</v>
-      </c>
-      <c r="C19" t="s">
-        <v>59</v>
-      </c>
-    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
         <v>64</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>65</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
@@ -1845,6 +1874,7 @@
     <row r="1002" ht="14.25" customHeight="1"/>
     <row r="1003" ht="14.25" customHeight="1"/>
     <row r="1004" ht="14.25" customHeight="1"/>
+    <row r="1005" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1856,7 +1886,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add new improve for multiple clientes
</commit_message>
<xml_diff>
--- a/STS IR Bot Dispatcher/Data/Config.xlsx
+++ b/STS IR Bot Dispatcher/Data/Config.xlsx
@@ -1,28 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://taxwarellc-my.sharepoint.com/personal/nahuel_delacruz_sovos_com/Documents/Desktop/Nahuel/Projects/STS Internal Review bot/STS IR Bot Dispatcher/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martin.martinez\Documents\github-IRBot\STS_InternalReviewBot\STS IR Bot Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{20A56275-A9E0-413C-960D-2EBDA3C80CF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E15444AD-EF3C-4031-982B-8DAB0123991D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B19A700A-BF1C-4797-95D5-692C8E5A6E51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7125" yWindow="4335" windowWidth="21600" windowHeight="11265" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
     <sheet name="Constants" sheetId="2" r:id="rId2"/>
     <sheet name="Assets" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="82">
   <si>
     <t>Name</t>
   </si>
@@ -264,6 +277,12 @@
   </si>
   <si>
     <t>\\somproddfs1.prod.sovos.org\depts\TaxReturnOutSourcing\Preparer\UIPathPublish\IR Bot Temp Files\InputFiles</t>
+  </si>
+  <si>
+    <t>PathDifferentPDriveFolder</t>
+  </si>
+  <si>
+    <t>\\10.250.52.158\Depts\TaxReturnOutSourcing\Preparer\UIPathPublish\IR Bot Temp Files\InputFiles</t>
   </si>
 </sst>
 </file>
@@ -653,10 +672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1004"/>
+  <dimension ref="A1:Z1005"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -811,57 +830,68 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:26" s="5" customFormat="1" ht="14.25" customHeight="1">
+    <row r="15" spans="1:26" s="6" customFormat="1" ht="14.25" customHeight="1">
       <c r="A15" s="5" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>75</v>
       </c>
+      <c r="D15" s="5"/>
     </row>
-    <row r="16" spans="1:26" s="6" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A16" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>77</v>
+    <row r="16" spans="1:26" s="5" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A16" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
       <c r="A17" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A18" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B18" s="6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A19" t="s">
-        <v>57</v>
-      </c>
-      <c r="B19" t="s">
-        <v>58</v>
-      </c>
-      <c r="C19" t="s">
-        <v>59</v>
-      </c>
-    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
         <v>64</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>65</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
@@ -1845,6 +1875,7 @@
     <row r="1002" ht="14.25" customHeight="1"/>
     <row r="1003" ht="14.25" customHeight="1"/>
     <row r="1004" ht="14.25" customHeight="1"/>
+    <row r="1005" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1856,7 +1887,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
config of multiple clients process
</commit_message>
<xml_diff>
--- a/STS IR Bot Dispatcher/Data/Config.xlsx
+++ b/STS IR Bot Dispatcher/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martin.martinez\Documents\github-IRBot\STS_InternalReviewBot\STS IR Bot Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F3C4234-F726-4C81-854F-2DAAEEC57946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B19A700A-BF1C-4797-95D5-692C8E5A6E51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -674,8 +674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -840,6 +840,7 @@
       <c r="C15" s="5" t="s">
         <v>75</v>
       </c>
+      <c r="D15" s="5"/>
     </row>
     <row r="16" spans="1:26" s="5" customFormat="1" ht="14.25" customHeight="1">
       <c r="A16" s="5" t="s">

</xml_diff>